<commit_message>
Update Pergantian Ban & Service Kendaraan
28/03/2024 15:45
</commit_message>
<xml_diff>
--- a/N 8624 UG HARUN.xlsx
+++ b/N 8624 UG HARUN.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
   <si>
     <t>No</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>15/1/2024</t>
+  </si>
+  <si>
+    <t>2 pc</t>
+  </si>
+  <si>
+    <t>27/03/2024</t>
   </si>
 </sst>
 </file>
@@ -605,8 +611,8 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,12 +974,25 @@
       <c r="A18" s="3">
         <v>14</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="1">
+        <v>425325</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18+10000</f>
+        <v>435325</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">

</xml_diff>